<commit_message>
update output for final week
</commit_message>
<xml_diff>
--- a/output/table1diamonds.xlsx
+++ b/output/table1diamonds.xlsx
@@ -56,73 +56,73 @@
     <t xml:space="preserve">     </t>
   </si>
   <si>
-    <t xml:space="preserve">      3 ( 2.0) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     16 (10.7) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     38 (25.3) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     41 (27.3) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     52 (34.7) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   0.82 (0.53)</t>
-  </si>
-  <si>
-    <t>4202.76 (4467.12)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      2 ( 2.8) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">      5 ( 6.9) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     18 (25.0) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     23 (31.9) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     24 (33.3) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   0.95 (0.57)</t>
-  </si>
-  <si>
-    <t>4825.92 (4825.38)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      1 ( 1.3) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     11 (14.1) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     20 (25.6) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     18 (23.1) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     28 (35.9) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   0.71 (0.46)</t>
-  </si>
-  <si>
-    <t>3627.54 (4055.41)</t>
+    <t xml:space="preserve">      4 ( 2.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     15 (10.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     33 (22.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     29 (19.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     69 (46.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.82 (0.54)</t>
+  </si>
+  <si>
+    <t>4356.75 (4876.03)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      2 ( 2.5) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      6 ( 7.4) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     17 (21.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     14 (17.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     42 (51.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.89 (0.59)</t>
+  </si>
+  <si>
+    <t>4557.68 (4972.55)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      2 ( 2.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      9 (13.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     16 (23.2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     15 (21.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     27 (39.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.75 (0.48)</t>
+  </si>
+  <si>
+    <t>4120.88 (4785.65)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Revert "update output for final week"
This reverts commit 1305494efbff18060e5d3dda5d026baaf88b0769.
</commit_message>
<xml_diff>
--- a/output/table1diamonds.xlsx
+++ b/output/table1diamonds.xlsx
@@ -56,73 +56,73 @@
     <t xml:space="preserve">     </t>
   </si>
   <si>
-    <t xml:space="preserve">      4 ( 2.7) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     15 (10.0) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     33 (22.0) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     29 (19.3) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     69 (46.0) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   0.82 (0.54)</t>
-  </si>
-  <si>
-    <t>4356.75 (4876.03)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      2 ( 2.5) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">      6 ( 7.4) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     17 (21.0) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     14 (17.3) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     42 (51.9) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   0.89 (0.59)</t>
-  </si>
-  <si>
-    <t>4557.68 (4972.55)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      2 ( 2.9) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">      9 (13.0) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     16 (23.2) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     15 (21.7) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     27 (39.1) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   0.75 (0.48)</t>
-  </si>
-  <si>
-    <t>4120.88 (4785.65)</t>
+    <t xml:space="preserve">      3 ( 2.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     16 (10.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     38 (25.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     41 (27.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     52 (34.7) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.82 (0.53)</t>
+  </si>
+  <si>
+    <t>4202.76 (4467.12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      2 ( 2.8) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      5 ( 6.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     18 (25.0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     23 (31.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     24 (33.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.95 (0.57)</t>
+  </si>
+  <si>
+    <t>4825.92 (4825.38)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      1 ( 1.3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     11 (14.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     20 (25.6) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     18 (23.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     28 (35.9) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0.71 (0.46)</t>
+  </si>
+  <si>
+    <t>3627.54 (4055.41)</t>
   </si>
 </sst>
 </file>

</xml_diff>